<commit_message>
fixed the issue with adding orders of the same day, modified the blankimport to contain information of the actual next rows of itself
</commit_message>
<xml_diff>
--- a/blankimport.xlsx
+++ b/blankimport.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Клиентский номер</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>Город / Регион отправления</t>
+  </si>
+  <si>
+    <t>Следующая строка (импорт):</t>
+  </si>
+  <si>
+    <t>Следующая строка (расписка):</t>
+  </si>
+  <si>
+    <t>То что ниже - не трогать!</t>
   </si>
 </sst>
 </file>
@@ -4964,10 +4973,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:N21"/>
+  <dimension ref="B3:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5112,10 +5121,25 @@
       </c>
       <c r="D21" s="7">
         <f ca="1">TODAY()</f>
-        <v>45952</v>
+        <v>45964</v>
       </c>
       <c r="F21" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>